<commit_message>
feat(importer): extend Excel importer and templates for richer word metadata
Add support for multi-column word lists with optional phonetic, definition,
example, tags, and image fields. Introduce robust whitespace and tag
sanitization utilities, deduplicate by normalized word text, and apply
consistent normalization across both importer and manual inputs.
Enhance upload prompt with a bundled template button, offline-open logic,
and clear help for new column usage. Update sample generator, test data,
and documentation to fully illustrate the expanded template.

BREAKING CHANGE: Legacy logic accepting words as plain strings will now
apply stricter normalization and deduplication. Users should review sample
templates and README for updated import conventions.
</commit_message>
<xml_diff>
--- a/data/单词列表.xlsx
+++ b/data/单词列表.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Vocabulary" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -435,6 +440,31 @@
           <t>单词</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>音标</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>释义</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>例句</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>标签</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>图片</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -442,349 +472,139 @@
           <t>apple</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>/ˈæpl/</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>n. 苹果；苹果树</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>An apple a day keeps the doctor away.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>水果, 基础词汇</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>banana</t>
-        </is>
-      </c>
+          <t>brave</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>/breɪv/</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>adj. 勇敢的；无畏的</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>The brave student volunteered to lead the team.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>品格, 励志</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cat</t>
-        </is>
-      </c>
+          <t>lantern</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>/ˈlæntərn/</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>n. 灯笼；提灯</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>We made a paper lantern for the Mid-Autumn Festival.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>节日, 手工制作</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dog</t>
-        </is>
-      </c>
+          <t>ocean</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>/ˈoʊʃn/</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>n. 海洋；大海</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Whales live in the deep ocean.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>自然, 动物</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>elephant</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>grape</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>house</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ice</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>juice</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>king</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>lion</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>monkey</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>nurse</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>orange</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>pig</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>queen</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>rabbit</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>sun</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>tiger</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>umbrella</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>violin</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>water</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>box</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>yellow</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>zebra</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>book</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>chair</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>desk</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>egg</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>flower</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>garden</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>hat</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>island</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>jacket</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>kite</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>lamp</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>moon</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>nest</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>ocean</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>pencil</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>quilt</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>river</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>star</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>tree</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>uniform</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>vase</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>window</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>fox</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>zoo</t>
-        </is>
-      </c>
+          <t>puzzle</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>/ˈpʌzl/</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>n. 谜题；拼图游戏</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>This English word puzzle is so much fun!</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>游戏, 课堂活动</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>